<commit_message>
updated prediction and stats for Aug & Sept
</commit_message>
<xml_diff>
--- a/restaurant_analytics/data/covers_data.xlsx
+++ b/restaurant_analytics/data/covers_data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29231"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cardi\Documents\git-repo\swe_dev\restaurant_analytics\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cardi\Documents\git-repo\swe_dev\restaurant_analytics\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E676F6E-2DE4-4E4E-8FEF-A86CCB856C99}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D40453D-8E81-49A1-924A-26B375F9E57E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="31125" yWindow="3135" windowWidth="21600" windowHeight="11295" xr2:uid="{12B37E6D-F535-4DBF-803D-25332F8C6D87}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{12B37E6D-F535-4DBF-803D-25332F8C6D87}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="518" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="582" uniqueCount="23">
   <si>
     <t>day</t>
   </si>
@@ -270,7 +270,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -298,15 +298,16 @@
     <xf numFmtId="3" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="14" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="14" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -641,11 +642,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{18DA2224-86A9-4CCC-80BA-0DF4A623F9C3}">
-  <dimension ref="A1:K508"/>
+  <dimension ref="A1:K573"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A20" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="M22" sqref="M22"/>
+      <pane ySplit="1" topLeftCell="A544" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="H558" sqref="H558"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -13347,7 +13348,7 @@
       <c r="B447">
         <v>446</v>
       </c>
-      <c r="C447" s="10">
+      <c r="C447" s="18">
         <v>45818</v>
       </c>
       <c r="D447" s="16">
@@ -13373,7 +13374,7 @@
       <c r="B448">
         <v>447</v>
       </c>
-      <c r="C448" s="17">
+      <c r="C448" s="19">
         <v>45819</v>
       </c>
       <c r="D448" s="16">
@@ -13399,7 +13400,7 @@
       <c r="B449">
         <v>448</v>
       </c>
-      <c r="C449" s="17">
+      <c r="C449" s="19">
         <v>45820</v>
       </c>
       <c r="D449" s="16">
@@ -13425,7 +13426,7 @@
       <c r="B450">
         <v>449</v>
       </c>
-      <c r="C450" s="17">
+      <c r="C450" s="19">
         <v>45821</v>
       </c>
       <c r="D450" s="16">
@@ -13451,7 +13452,7 @@
       <c r="B451">
         <v>450</v>
       </c>
-      <c r="C451" s="17">
+      <c r="C451" s="19">
         <v>45822</v>
       </c>
       <c r="D451" s="16">
@@ -13477,7 +13478,7 @@
       <c r="B452">
         <v>451</v>
       </c>
-      <c r="C452" s="17">
+      <c r="C452" s="19">
         <v>45823</v>
       </c>
       <c r="D452" s="16">
@@ -13503,7 +13504,7 @@
       <c r="B453">
         <v>452</v>
       </c>
-      <c r="C453" s="17">
+      <c r="C453" s="19">
         <v>45824</v>
       </c>
       <c r="D453" s="16">
@@ -13529,7 +13530,7 @@
       <c r="B454">
         <v>453</v>
       </c>
-      <c r="C454" s="17">
+      <c r="C454" s="19">
         <v>45825</v>
       </c>
       <c r="D454" s="16">
@@ -13555,7 +13556,7 @@
       <c r="B455">
         <v>454</v>
       </c>
-      <c r="C455" s="17">
+      <c r="C455" s="19">
         <v>45826</v>
       </c>
       <c r="D455" s="16">
@@ -13581,7 +13582,7 @@
       <c r="B456">
         <v>455</v>
       </c>
-      <c r="C456" s="17">
+      <c r="C456" s="19">
         <v>45827</v>
       </c>
       <c r="D456" s="16">
@@ -13607,7 +13608,7 @@
       <c r="B457">
         <v>456</v>
       </c>
-      <c r="C457" s="17">
+      <c r="C457" s="19">
         <v>45828</v>
       </c>
       <c r="D457" s="16">
@@ -13633,7 +13634,7 @@
       <c r="B458">
         <v>457</v>
       </c>
-      <c r="C458" s="17">
+      <c r="C458" s="19">
         <v>45829</v>
       </c>
       <c r="D458" s="16">
@@ -13659,7 +13660,7 @@
       <c r="B459">
         <v>458</v>
       </c>
-      <c r="C459" s="17">
+      <c r="C459" s="19">
         <v>45830</v>
       </c>
       <c r="D459" s="16">
@@ -13685,7 +13686,7 @@
       <c r="B460">
         <v>459</v>
       </c>
-      <c r="C460" s="17">
+      <c r="C460" s="19">
         <v>45831</v>
       </c>
       <c r="D460" s="16">
@@ -13711,7 +13712,7 @@
       <c r="B461">
         <v>460</v>
       </c>
-      <c r="C461" s="17">
+      <c r="C461" s="19">
         <v>45832</v>
       </c>
       <c r="D461" s="16">
@@ -13737,7 +13738,7 @@
       <c r="B462">
         <v>461</v>
       </c>
-      <c r="C462" s="17">
+      <c r="C462" s="19">
         <v>45833</v>
       </c>
       <c r="D462" s="16">
@@ -13763,7 +13764,7 @@
       <c r="B463">
         <v>462</v>
       </c>
-      <c r="C463" s="17">
+      <c r="C463" s="19">
         <v>45834</v>
       </c>
       <c r="D463" s="16">
@@ -13789,7 +13790,7 @@
       <c r="B464">
         <v>463</v>
       </c>
-      <c r="C464" s="17">
+      <c r="C464" s="19">
         <v>45835</v>
       </c>
       <c r="D464" s="16">
@@ -13815,7 +13816,7 @@
       <c r="B465">
         <v>464</v>
       </c>
-      <c r="C465" s="17">
+      <c r="C465" s="19">
         <v>45836</v>
       </c>
       <c r="D465" s="16">
@@ -13841,7 +13842,7 @@
       <c r="B466">
         <v>465</v>
       </c>
-      <c r="C466" s="17">
+      <c r="C466" s="19">
         <v>45837</v>
       </c>
       <c r="D466" s="16">
@@ -13867,7 +13868,7 @@
       <c r="B467">
         <v>466</v>
       </c>
-      <c r="C467" s="17">
+      <c r="C467" s="19">
         <v>45838</v>
       </c>
       <c r="D467" s="16">
@@ -13893,10 +13894,10 @@
       <c r="B468">
         <v>467</v>
       </c>
-      <c r="C468" s="17">
+      <c r="C468" s="19">
         <v>45839</v>
       </c>
-      <c r="D468" s="18">
+      <c r="D468" s="17">
         <v>82</v>
       </c>
       <c r="E468">
@@ -13919,10 +13920,10 @@
       <c r="B469">
         <v>468</v>
       </c>
-      <c r="C469" s="17">
+      <c r="C469" s="19">
         <v>45840</v>
       </c>
-      <c r="D469" s="18">
+      <c r="D469" s="17">
         <v>69</v>
       </c>
       <c r="E469">
@@ -13945,10 +13946,10 @@
       <c r="B470">
         <v>469</v>
       </c>
-      <c r="C470" s="17">
+      <c r="C470" s="19">
         <v>45841</v>
       </c>
-      <c r="D470" s="18">
+      <c r="D470" s="17">
         <v>137</v>
       </c>
       <c r="E470">
@@ -13971,10 +13972,10 @@
       <c r="B471">
         <v>470</v>
       </c>
-      <c r="C471" s="17">
+      <c r="C471" s="19">
         <v>45842</v>
       </c>
-      <c r="D471" s="18">
+      <c r="D471" s="17">
         <v>0</v>
       </c>
       <c r="E471">
@@ -13997,10 +13998,10 @@
       <c r="B472">
         <v>471</v>
       </c>
-      <c r="C472" s="17">
+      <c r="C472" s="19">
         <v>45843</v>
       </c>
-      <c r="D472" s="18">
+      <c r="D472" s="17">
         <v>150</v>
       </c>
       <c r="E472">
@@ -14023,10 +14024,10 @@
       <c r="B473" s="13">
         <v>472</v>
       </c>
-      <c r="C473" s="19">
+      <c r="C473" s="14">
         <v>45844</v>
       </c>
-      <c r="D473" s="18">
+      <c r="D473" s="17">
         <v>44</v>
       </c>
       <c r="E473">
@@ -14049,10 +14050,10 @@
       <c r="B474" s="13">
         <v>473</v>
       </c>
-      <c r="C474" s="19">
+      <c r="C474" s="14">
         <v>45845</v>
       </c>
-      <c r="D474" s="18">
+      <c r="D474" s="17">
         <v>52</v>
       </c>
       <c r="E474">
@@ -14075,10 +14076,10 @@
       <c r="B475" s="13">
         <v>474</v>
       </c>
-      <c r="C475" s="19">
+      <c r="C475" s="14">
         <v>45846</v>
       </c>
-      <c r="D475" s="18">
+      <c r="D475" s="17">
         <v>68</v>
       </c>
       <c r="E475">
@@ -14101,10 +14102,10 @@
       <c r="B476" s="13">
         <v>475</v>
       </c>
-      <c r="C476" s="19">
+      <c r="C476" s="14">
         <v>45847</v>
       </c>
-      <c r="D476" s="18">
+      <c r="D476" s="17">
         <v>64</v>
       </c>
       <c r="E476">
@@ -14127,10 +14128,10 @@
       <c r="B477" s="13">
         <v>476</v>
       </c>
-      <c r="C477" s="19">
+      <c r="C477" s="14">
         <v>45848</v>
       </c>
-      <c r="D477" s="18">
+      <c r="D477" s="17">
         <v>85</v>
       </c>
       <c r="E477">
@@ -14153,7 +14154,7 @@
       <c r="B478" s="13">
         <v>477</v>
       </c>
-      <c r="C478" s="19">
+      <c r="C478" s="14">
         <v>45849</v>
       </c>
       <c r="D478">
@@ -14179,7 +14180,7 @@
       <c r="B479" s="13">
         <v>478</v>
       </c>
-      <c r="C479" s="19">
+      <c r="C479" s="14">
         <v>45850</v>
       </c>
       <c r="D479">
@@ -14205,7 +14206,7 @@
       <c r="B480" s="13">
         <v>479</v>
       </c>
-      <c r="C480" s="19">
+      <c r="C480" s="14">
         <v>45851</v>
       </c>
       <c r="D480">
@@ -14231,7 +14232,7 @@
       <c r="B481" s="13">
         <v>480</v>
       </c>
-      <c r="C481" s="19">
+      <c r="C481" s="14">
         <v>45852</v>
       </c>
       <c r="D481">
@@ -14257,7 +14258,7 @@
       <c r="B482" s="13">
         <v>481</v>
       </c>
-      <c r="C482" s="19">
+      <c r="C482" s="14">
         <v>45853</v>
       </c>
       <c r="D482">
@@ -14283,7 +14284,7 @@
       <c r="B483" s="13">
         <v>482</v>
       </c>
-      <c r="C483" s="19">
+      <c r="C483" s="14">
         <v>45854</v>
       </c>
       <c r="D483">
@@ -14309,7 +14310,7 @@
       <c r="B484" s="13">
         <v>483</v>
       </c>
-      <c r="C484" s="19">
+      <c r="C484" s="14">
         <v>45855</v>
       </c>
       <c r="D484">
@@ -14335,7 +14336,7 @@
       <c r="B485" s="13">
         <v>484</v>
       </c>
-      <c r="C485" s="19">
+      <c r="C485" s="14">
         <v>45856</v>
       </c>
       <c r="D485">
@@ -14361,7 +14362,7 @@
       <c r="B486" s="13">
         <v>485</v>
       </c>
-      <c r="C486" s="19">
+      <c r="C486" s="14">
         <v>45857</v>
       </c>
       <c r="D486">
@@ -14387,7 +14388,7 @@
       <c r="B487" s="13">
         <v>486</v>
       </c>
-      <c r="C487" s="19">
+      <c r="C487" s="14">
         <v>45858</v>
       </c>
       <c r="D487">
@@ -14413,7 +14414,7 @@
       <c r="B488" s="13">
         <v>487</v>
       </c>
-      <c r="C488" s="19">
+      <c r="C488" s="14">
         <v>45859</v>
       </c>
       <c r="D488">
@@ -14439,7 +14440,7 @@
       <c r="B489" s="13">
         <v>488</v>
       </c>
-      <c r="C489" s="19">
+      <c r="C489" s="14">
         <v>45860</v>
       </c>
       <c r="D489">
@@ -14465,7 +14466,7 @@
       <c r="B490" s="13">
         <v>489</v>
       </c>
-      <c r="C490" s="19">
+      <c r="C490" s="14">
         <v>45861</v>
       </c>
       <c r="D490">
@@ -14491,7 +14492,7 @@
       <c r="B491" s="13">
         <v>490</v>
       </c>
-      <c r="C491" s="19">
+      <c r="C491" s="14">
         <v>45862</v>
       </c>
       <c r="D491">
@@ -14517,7 +14518,7 @@
       <c r="B492" s="13">
         <v>491</v>
       </c>
-      <c r="C492" s="19">
+      <c r="C492" s="14">
         <v>45863</v>
       </c>
       <c r="D492">
@@ -14543,7 +14544,7 @@
       <c r="B493" s="13">
         <v>492</v>
       </c>
-      <c r="C493" s="19">
+      <c r="C493" s="14">
         <v>45864</v>
       </c>
       <c r="D493">
@@ -14569,7 +14570,7 @@
       <c r="B494" s="13">
         <v>493</v>
       </c>
-      <c r="C494" s="19">
+      <c r="C494" s="14">
         <v>45865</v>
       </c>
       <c r="D494">
@@ -14595,7 +14596,7 @@
       <c r="B495" s="13">
         <v>494</v>
       </c>
-      <c r="C495" s="19">
+      <c r="C495" s="14">
         <v>45866</v>
       </c>
       <c r="D495">
@@ -14621,7 +14622,7 @@
       <c r="B496" s="13">
         <v>495</v>
       </c>
-      <c r="C496" s="19">
+      <c r="C496" s="14">
         <v>45867</v>
       </c>
       <c r="D496">
@@ -14647,7 +14648,7 @@
       <c r="B497" s="13">
         <v>496</v>
       </c>
-      <c r="C497" s="19">
+      <c r="C497" s="14">
         <v>45868</v>
       </c>
       <c r="D497">
@@ -14673,7 +14674,7 @@
       <c r="B498" s="13">
         <v>497</v>
       </c>
-      <c r="C498" s="19">
+      <c r="C498" s="14">
         <v>45869</v>
       </c>
       <c r="D498">
@@ -14699,7 +14700,7 @@
       <c r="B499" s="13">
         <v>498</v>
       </c>
-      <c r="C499" s="19">
+      <c r="C499" s="14">
         <v>45870</v>
       </c>
       <c r="D499">
@@ -14725,7 +14726,7 @@
       <c r="B500" s="13">
         <v>499</v>
       </c>
-      <c r="C500" s="19">
+      <c r="C500" s="14">
         <v>45871</v>
       </c>
       <c r="D500">
@@ -14751,7 +14752,7 @@
       <c r="B501" s="13">
         <v>500</v>
       </c>
-      <c r="C501" s="19">
+      <c r="C501" s="14">
         <v>45872</v>
       </c>
       <c r="D501">
@@ -14777,7 +14778,7 @@
       <c r="B502" s="13">
         <v>501</v>
       </c>
-      <c r="C502" s="19">
+      <c r="C502" s="14">
         <v>45873</v>
       </c>
       <c r="D502">
@@ -14803,7 +14804,7 @@
       <c r="B503" s="13">
         <v>502</v>
       </c>
-      <c r="C503" s="19">
+      <c r="C503" s="14">
         <v>45874</v>
       </c>
       <c r="D503">
@@ -14811,7 +14812,7 @@
       </c>
       <c r="E503">
         <f t="shared" si="31"/>
-        <v>37.5</v>
+        <v>7.5</v>
       </c>
       <c r="F503">
         <f t="shared" si="32"/>
@@ -14823,19 +14824,1686 @@
       </c>
     </row>
     <row r="504" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A504" s="8"/>
+      <c r="A504" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="B504" s="13">
+        <v>503</v>
+      </c>
+      <c r="C504" s="14">
+        <v>45875</v>
+      </c>
+      <c r="D504">
+        <v>60</v>
+      </c>
+      <c r="E504">
+        <f t="shared" ref="E504:E567" si="34">(D503-D505)/2</f>
+        <v>-21</v>
+      </c>
+      <c r="F504">
+        <f t="shared" ref="F504:F567" si="35">IF(AND(D504&gt;D503,D504&gt;D505,D504&gt;100),D504,0)</f>
+        <v>0</v>
+      </c>
+      <c r="G504">
+        <f t="shared" ref="G504:G567" si="36">IF(D504&gt;100,D504,0)</f>
+        <v>0</v>
+      </c>
     </row>
     <row r="505" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A505" s="8"/>
+      <c r="A505" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="B505" s="13">
+        <v>504</v>
+      </c>
+      <c r="C505" s="14">
+        <v>45876</v>
+      </c>
+      <c r="D505">
+        <v>91</v>
+      </c>
+      <c r="E505">
+        <f t="shared" si="34"/>
+        <v>-38</v>
+      </c>
+      <c r="F505">
+        <f t="shared" si="35"/>
+        <v>0</v>
+      </c>
+      <c r="G505">
+        <f t="shared" si="36"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="506" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A506" s="8"/>
+      <c r="A506" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="B506" s="13">
+        <v>505</v>
+      </c>
+      <c r="C506" s="14">
+        <v>45877</v>
+      </c>
+      <c r="D506">
+        <v>136</v>
+      </c>
+      <c r="E506">
+        <f t="shared" si="34"/>
+        <v>-34</v>
+      </c>
+      <c r="F506">
+        <f t="shared" si="35"/>
+        <v>0</v>
+      </c>
+      <c r="G506">
+        <f t="shared" si="36"/>
+        <v>136</v>
+      </c>
     </row>
     <row r="507" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A507" s="8"/>
+      <c r="A507" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="B507" s="13">
+        <v>506</v>
+      </c>
+      <c r="C507" s="14">
+        <v>45878</v>
+      </c>
+      <c r="D507">
+        <v>159</v>
+      </c>
+      <c r="E507">
+        <f t="shared" si="34"/>
+        <v>31.5</v>
+      </c>
+      <c r="F507">
+        <f t="shared" si="35"/>
+        <v>159</v>
+      </c>
+      <c r="G507">
+        <f t="shared" si="36"/>
+        <v>159</v>
+      </c>
     </row>
     <row r="508" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A508" s="8"/>
+      <c r="A508" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="B508" s="13">
+        <v>507</v>
+      </c>
+      <c r="C508" s="14">
+        <v>45879</v>
+      </c>
+      <c r="D508">
+        <v>73</v>
+      </c>
+      <c r="E508">
+        <f t="shared" si="34"/>
+        <v>48</v>
+      </c>
+      <c r="F508">
+        <f t="shared" si="35"/>
+        <v>0</v>
+      </c>
+      <c r="G508">
+        <f t="shared" si="36"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="509" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A509" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="B509" s="13">
+        <v>508</v>
+      </c>
+      <c r="C509" s="14">
+        <v>45880</v>
+      </c>
+      <c r="D509">
+        <v>63</v>
+      </c>
+      <c r="E509">
+        <f t="shared" si="34"/>
+        <v>9</v>
+      </c>
+      <c r="F509">
+        <f t="shared" si="35"/>
+        <v>0</v>
+      </c>
+      <c r="G509">
+        <f t="shared" si="36"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="510" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A510" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="B510" s="13">
+        <v>509</v>
+      </c>
+      <c r="C510" s="14">
+        <v>45881</v>
+      </c>
+      <c r="D510">
+        <v>55</v>
+      </c>
+      <c r="E510">
+        <f t="shared" si="34"/>
+        <v>4.5</v>
+      </c>
+      <c r="F510">
+        <f t="shared" si="35"/>
+        <v>0</v>
+      </c>
+      <c r="G510">
+        <f t="shared" si="36"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="511" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A511" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="B511" s="13">
+        <v>510</v>
+      </c>
+      <c r="C511" s="14">
+        <v>45882</v>
+      </c>
+      <c r="D511">
+        <v>54</v>
+      </c>
+      <c r="E511">
+        <f t="shared" si="34"/>
+        <v>-13.5</v>
+      </c>
+      <c r="F511">
+        <f t="shared" si="35"/>
+        <v>0</v>
+      </c>
+      <c r="G511">
+        <f t="shared" si="36"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="512" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A512" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="B512" s="13">
+        <v>511</v>
+      </c>
+      <c r="C512" s="14">
+        <v>45883</v>
+      </c>
+      <c r="D512" s="17">
+        <v>82</v>
+      </c>
+      <c r="E512">
+        <f t="shared" si="34"/>
+        <v>-43</v>
+      </c>
+      <c r="F512">
+        <f t="shared" si="35"/>
+        <v>0</v>
+      </c>
+      <c r="G512">
+        <f t="shared" si="36"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="513" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A513" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="B513" s="13">
+        <v>512</v>
+      </c>
+      <c r="C513" s="14">
+        <v>45884</v>
+      </c>
+      <c r="D513" s="17">
+        <v>140</v>
+      </c>
+      <c r="E513">
+        <f t="shared" si="34"/>
+        <v>-40</v>
+      </c>
+      <c r="F513">
+        <f t="shared" si="35"/>
+        <v>0</v>
+      </c>
+      <c r="G513">
+        <f t="shared" si="36"/>
+        <v>140</v>
+      </c>
+    </row>
+    <row r="514" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A514" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="B514" s="13">
+        <v>513</v>
+      </c>
+      <c r="C514" s="14">
+        <v>45885</v>
+      </c>
+      <c r="D514" s="17">
+        <v>162</v>
+      </c>
+      <c r="E514">
+        <f t="shared" si="34"/>
+        <v>24</v>
+      </c>
+      <c r="F514">
+        <f t="shared" si="35"/>
+        <v>162</v>
+      </c>
+      <c r="G514">
+        <f t="shared" si="36"/>
+        <v>162</v>
+      </c>
+    </row>
+    <row r="515" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A515" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="B515" s="13">
+        <v>514</v>
+      </c>
+      <c r="C515" s="14">
+        <v>45886</v>
+      </c>
+      <c r="D515" s="17">
+        <v>92</v>
+      </c>
+      <c r="E515">
+        <f t="shared" si="34"/>
+        <v>38</v>
+      </c>
+      <c r="F515">
+        <f t="shared" si="35"/>
+        <v>0</v>
+      </c>
+      <c r="G515">
+        <f t="shared" si="36"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="516" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A516" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="B516" s="13">
+        <v>515</v>
+      </c>
+      <c r="C516" s="14">
+        <v>45887</v>
+      </c>
+      <c r="D516" s="17">
+        <v>86</v>
+      </c>
+      <c r="E516">
+        <f t="shared" si="34"/>
+        <v>15</v>
+      </c>
+      <c r="F516">
+        <f t="shared" si="35"/>
+        <v>0</v>
+      </c>
+      <c r="G516">
+        <f t="shared" si="36"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="517" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A517" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="B517" s="13">
+        <v>516</v>
+      </c>
+      <c r="C517" s="14">
+        <v>45888</v>
+      </c>
+      <c r="D517" s="17">
+        <v>62</v>
+      </c>
+      <c r="E517">
+        <f t="shared" si="34"/>
+        <v>3.5</v>
+      </c>
+      <c r="F517">
+        <f t="shared" si="35"/>
+        <v>0</v>
+      </c>
+      <c r="G517">
+        <f t="shared" si="36"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="518" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A518" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="B518" s="13">
+        <v>517</v>
+      </c>
+      <c r="C518" s="14">
+        <v>45889</v>
+      </c>
+      <c r="D518" s="17">
+        <v>79</v>
+      </c>
+      <c r="E518">
+        <f t="shared" si="34"/>
+        <v>-33</v>
+      </c>
+      <c r="F518">
+        <f t="shared" si="35"/>
+        <v>0</v>
+      </c>
+      <c r="G518">
+        <f t="shared" si="36"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="519" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A519" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="B519" s="13">
+        <v>518</v>
+      </c>
+      <c r="C519" s="14">
+        <v>45890</v>
+      </c>
+      <c r="D519" s="17">
+        <v>128</v>
+      </c>
+      <c r="E519">
+        <f t="shared" si="34"/>
+        <v>-39</v>
+      </c>
+      <c r="F519">
+        <f t="shared" si="35"/>
+        <v>0</v>
+      </c>
+      <c r="G519">
+        <f t="shared" si="36"/>
+        <v>128</v>
+      </c>
+    </row>
+    <row r="520" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A520" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="B520" s="13">
+        <v>519</v>
+      </c>
+      <c r="C520" s="14">
+        <v>45891</v>
+      </c>
+      <c r="D520" s="17">
+        <v>157</v>
+      </c>
+      <c r="E520">
+        <f t="shared" si="34"/>
+        <v>-44</v>
+      </c>
+      <c r="F520">
+        <f t="shared" si="35"/>
+        <v>0</v>
+      </c>
+      <c r="G520">
+        <f t="shared" si="36"/>
+        <v>157</v>
+      </c>
+    </row>
+    <row r="521" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A521" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="B521" s="13">
+        <v>520</v>
+      </c>
+      <c r="C521" s="14">
+        <v>45892</v>
+      </c>
+      <c r="D521" s="17">
+        <v>216</v>
+      </c>
+      <c r="E521">
+        <f t="shared" si="34"/>
+        <v>43</v>
+      </c>
+      <c r="F521">
+        <f t="shared" si="35"/>
+        <v>216</v>
+      </c>
+      <c r="G521">
+        <f t="shared" si="36"/>
+        <v>216</v>
+      </c>
+    </row>
+    <row r="522" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A522" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="B522" s="13">
+        <v>521</v>
+      </c>
+      <c r="C522" s="14">
+        <v>45893</v>
+      </c>
+      <c r="D522" s="17">
+        <v>71</v>
+      </c>
+      <c r="E522">
+        <f t="shared" si="34"/>
+        <v>91</v>
+      </c>
+      <c r="F522">
+        <f t="shared" si="35"/>
+        <v>0</v>
+      </c>
+      <c r="G522">
+        <f t="shared" si="36"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="523" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A523" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="B523" s="13">
+        <v>522</v>
+      </c>
+      <c r="C523" s="14">
+        <v>45894</v>
+      </c>
+      <c r="D523" s="17">
+        <v>34</v>
+      </c>
+      <c r="E523">
+        <f t="shared" si="34"/>
+        <v>-3</v>
+      </c>
+      <c r="F523">
+        <f t="shared" si="35"/>
+        <v>0</v>
+      </c>
+      <c r="G523">
+        <f t="shared" si="36"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="524" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A524" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="B524" s="13">
+        <v>523</v>
+      </c>
+      <c r="C524" s="14">
+        <v>45895</v>
+      </c>
+      <c r="D524" s="17">
+        <v>77</v>
+      </c>
+      <c r="E524">
+        <f t="shared" si="34"/>
+        <v>-34</v>
+      </c>
+      <c r="F524">
+        <f t="shared" si="35"/>
+        <v>0</v>
+      </c>
+      <c r="G524">
+        <f t="shared" si="36"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="525" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A525" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="B525" s="13">
+        <v>524</v>
+      </c>
+      <c r="C525" s="14">
+        <v>45896</v>
+      </c>
+      <c r="D525" s="17">
+        <v>102</v>
+      </c>
+      <c r="E525">
+        <f t="shared" si="34"/>
+        <v>-4.5</v>
+      </c>
+      <c r="F525">
+        <f t="shared" si="35"/>
+        <v>102</v>
+      </c>
+      <c r="G525">
+        <f t="shared" si="36"/>
+        <v>102</v>
+      </c>
+    </row>
+    <row r="526" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A526" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="B526" s="13">
+        <v>525</v>
+      </c>
+      <c r="C526" s="14">
+        <v>45897</v>
+      </c>
+      <c r="D526" s="17">
+        <v>86</v>
+      </c>
+      <c r="E526">
+        <f t="shared" si="34"/>
+        <v>-19</v>
+      </c>
+      <c r="F526">
+        <f t="shared" si="35"/>
+        <v>0</v>
+      </c>
+      <c r="G526">
+        <f t="shared" si="36"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="527" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A527" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="B527" s="13">
+        <v>526</v>
+      </c>
+      <c r="C527" s="14">
+        <v>45898</v>
+      </c>
+      <c r="D527" s="17">
+        <v>140</v>
+      </c>
+      <c r="E527">
+        <f t="shared" si="34"/>
+        <v>-39</v>
+      </c>
+      <c r="F527">
+        <f t="shared" si="35"/>
+        <v>0</v>
+      </c>
+      <c r="G527">
+        <f t="shared" si="36"/>
+        <v>140</v>
+      </c>
+    </row>
+    <row r="528" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A528" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="B528" s="13">
+        <v>527</v>
+      </c>
+      <c r="C528" s="14">
+        <v>45899</v>
+      </c>
+      <c r="D528" s="17">
+        <v>164</v>
+      </c>
+      <c r="E528">
+        <f t="shared" si="34"/>
+        <v>36</v>
+      </c>
+      <c r="F528">
+        <f t="shared" si="35"/>
+        <v>164</v>
+      </c>
+      <c r="G528">
+        <f t="shared" si="36"/>
+        <v>164</v>
+      </c>
+    </row>
+    <row r="529" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A529" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="B529" s="13">
+        <v>528</v>
+      </c>
+      <c r="C529" s="14">
+        <v>45900</v>
+      </c>
+      <c r="D529" s="17">
+        <v>68</v>
+      </c>
+      <c r="E529">
+        <f t="shared" si="34"/>
+        <v>82</v>
+      </c>
+      <c r="F529">
+        <f t="shared" si="35"/>
+        <v>0</v>
+      </c>
+      <c r="G529">
+        <f t="shared" si="36"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="530" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A530" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="B530" s="13">
+        <v>529</v>
+      </c>
+      <c r="C530" s="14">
+        <v>45901</v>
+      </c>
+      <c r="D530" s="17">
+        <v>0</v>
+      </c>
+      <c r="E530">
+        <f t="shared" si="34"/>
+        <v>11.5</v>
+      </c>
+      <c r="F530">
+        <f t="shared" si="35"/>
+        <v>0</v>
+      </c>
+      <c r="G530">
+        <f t="shared" si="36"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="531" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A531" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="B531" s="13">
+        <v>530</v>
+      </c>
+      <c r="C531" s="14">
+        <v>45902</v>
+      </c>
+      <c r="D531" s="17">
+        <v>45</v>
+      </c>
+      <c r="E531">
+        <f t="shared" si="34"/>
+        <v>-18</v>
+      </c>
+      <c r="F531">
+        <f t="shared" si="35"/>
+        <v>0</v>
+      </c>
+      <c r="G531">
+        <f t="shared" si="36"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="532" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A532" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="B532" s="13">
+        <v>531</v>
+      </c>
+      <c r="C532" s="14">
+        <v>45903</v>
+      </c>
+      <c r="D532" s="17">
+        <v>36</v>
+      </c>
+      <c r="E532">
+        <f t="shared" si="34"/>
+        <v>-7</v>
+      </c>
+      <c r="F532">
+        <f t="shared" si="35"/>
+        <v>0</v>
+      </c>
+      <c r="G532">
+        <f t="shared" si="36"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="533" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A533" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="B533" s="13">
+        <v>532</v>
+      </c>
+      <c r="C533" s="14">
+        <v>45904</v>
+      </c>
+      <c r="D533" s="17">
+        <v>59</v>
+      </c>
+      <c r="E533">
+        <f t="shared" si="34"/>
+        <v>-35.5</v>
+      </c>
+      <c r="F533">
+        <f t="shared" si="35"/>
+        <v>0</v>
+      </c>
+      <c r="G533">
+        <f t="shared" si="36"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="534" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A534" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="B534" s="13">
+        <v>533</v>
+      </c>
+      <c r="C534" s="14">
+        <v>45905</v>
+      </c>
+      <c r="D534" s="17">
+        <v>107</v>
+      </c>
+      <c r="E534">
+        <f t="shared" si="34"/>
+        <v>-46.5</v>
+      </c>
+      <c r="F534">
+        <f t="shared" si="35"/>
+        <v>0</v>
+      </c>
+      <c r="G534">
+        <f t="shared" si="36"/>
+        <v>107</v>
+      </c>
+    </row>
+    <row r="535" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A535" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="B535" s="13">
+        <v>534</v>
+      </c>
+      <c r="C535" s="14">
+        <v>45906</v>
+      </c>
+      <c r="D535" s="17">
+        <v>152</v>
+      </c>
+      <c r="E535">
+        <f t="shared" si="34"/>
+        <v>30.5</v>
+      </c>
+      <c r="F535">
+        <f t="shared" si="35"/>
+        <v>152</v>
+      </c>
+      <c r="G535">
+        <f t="shared" si="36"/>
+        <v>152</v>
+      </c>
+    </row>
+    <row r="536" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A536" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="B536" s="13">
+        <v>535</v>
+      </c>
+      <c r="C536" s="14">
+        <v>45907</v>
+      </c>
+      <c r="D536" s="17">
+        <v>46</v>
+      </c>
+      <c r="E536">
+        <f t="shared" si="34"/>
+        <v>56.5</v>
+      </c>
+      <c r="F536">
+        <f t="shared" si="35"/>
+        <v>0</v>
+      </c>
+      <c r="G536">
+        <f t="shared" si="36"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="537" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A537" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="B537" s="13">
+        <v>536</v>
+      </c>
+      <c r="C537" s="14">
+        <v>45908</v>
+      </c>
+      <c r="D537" s="17">
+        <v>39</v>
+      </c>
+      <c r="E537">
+        <f t="shared" si="34"/>
+        <v>-6</v>
+      </c>
+      <c r="F537">
+        <f t="shared" si="35"/>
+        <v>0</v>
+      </c>
+      <c r="G537">
+        <f t="shared" si="36"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="538" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A538" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="B538" s="13">
+        <v>537</v>
+      </c>
+      <c r="C538" s="14">
+        <v>45909</v>
+      </c>
+      <c r="D538" s="17">
+        <v>58</v>
+      </c>
+      <c r="E538">
+        <f t="shared" si="34"/>
+        <v>-22</v>
+      </c>
+      <c r="F538">
+        <f t="shared" si="35"/>
+        <v>0</v>
+      </c>
+      <c r="G538">
+        <f t="shared" si="36"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="539" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A539" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="B539" s="13">
+        <v>538</v>
+      </c>
+      <c r="C539" s="14">
+        <v>45910</v>
+      </c>
+      <c r="D539" s="17">
+        <v>83</v>
+      </c>
+      <c r="E539">
+        <f t="shared" si="34"/>
+        <v>-11.5</v>
+      </c>
+      <c r="F539">
+        <f t="shared" si="35"/>
+        <v>0</v>
+      </c>
+      <c r="G539">
+        <f t="shared" si="36"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="540" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A540" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="B540" s="13">
+        <v>539</v>
+      </c>
+      <c r="C540" s="14">
+        <v>45911</v>
+      </c>
+      <c r="D540" s="17">
+        <v>81</v>
+      </c>
+      <c r="E540">
+        <f t="shared" si="34"/>
+        <v>-17</v>
+      </c>
+      <c r="F540">
+        <f t="shared" si="35"/>
+        <v>0</v>
+      </c>
+      <c r="G540">
+        <f t="shared" si="36"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="541" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A541" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="B541" s="13">
+        <v>540</v>
+      </c>
+      <c r="C541" s="14">
+        <v>45912</v>
+      </c>
+      <c r="D541" s="17">
+        <v>117</v>
+      </c>
+      <c r="E541">
+        <f t="shared" si="34"/>
+        <v>-33.5</v>
+      </c>
+      <c r="F541">
+        <f t="shared" si="35"/>
+        <v>0</v>
+      </c>
+      <c r="G541">
+        <f t="shared" si="36"/>
+        <v>117</v>
+      </c>
+    </row>
+    <row r="542" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A542" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="B542" s="13">
+        <v>541</v>
+      </c>
+      <c r="C542" s="14">
+        <v>45913</v>
+      </c>
+      <c r="D542" s="17">
+        <v>148</v>
+      </c>
+      <c r="E542">
+        <f t="shared" si="34"/>
+        <v>33</v>
+      </c>
+      <c r="F542">
+        <f t="shared" si="35"/>
+        <v>148</v>
+      </c>
+      <c r="G542">
+        <f t="shared" si="36"/>
+        <v>148</v>
+      </c>
+    </row>
+    <row r="543" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A543" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="B543" s="13">
+        <v>542</v>
+      </c>
+      <c r="C543" s="14">
+        <v>45914</v>
+      </c>
+      <c r="D543" s="17">
+        <v>51</v>
+      </c>
+      <c r="E543">
+        <f t="shared" si="34"/>
+        <v>35.5</v>
+      </c>
+      <c r="F543">
+        <f t="shared" si="35"/>
+        <v>0</v>
+      </c>
+      <c r="G543">
+        <f t="shared" si="36"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="544" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A544" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="B544" s="13">
+        <v>543</v>
+      </c>
+      <c r="C544" s="14">
+        <v>45915</v>
+      </c>
+      <c r="D544" s="17">
+        <v>77</v>
+      </c>
+      <c r="E544">
+        <f t="shared" si="34"/>
+        <v>-14.5</v>
+      </c>
+      <c r="F544">
+        <f t="shared" si="35"/>
+        <v>0</v>
+      </c>
+      <c r="G544">
+        <f t="shared" si="36"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="545" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A545" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="B545" s="13">
+        <v>544</v>
+      </c>
+      <c r="C545" s="14">
+        <v>45916</v>
+      </c>
+      <c r="D545" s="17">
+        <v>80</v>
+      </c>
+      <c r="E545">
+        <f t="shared" si="34"/>
+        <v>4</v>
+      </c>
+      <c r="F545">
+        <f t="shared" si="35"/>
+        <v>0</v>
+      </c>
+      <c r="G545">
+        <f t="shared" si="36"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="546" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A546" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="B546" s="13">
+        <v>545</v>
+      </c>
+      <c r="C546" s="14">
+        <v>45917</v>
+      </c>
+      <c r="D546" s="17">
+        <v>69</v>
+      </c>
+      <c r="E546">
+        <f t="shared" si="34"/>
+        <v>-9</v>
+      </c>
+      <c r="F546">
+        <f t="shared" si="35"/>
+        <v>0</v>
+      </c>
+      <c r="G546">
+        <f t="shared" si="36"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="547" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A547" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="B547" s="13">
+        <v>546</v>
+      </c>
+      <c r="C547" s="14">
+        <v>45918</v>
+      </c>
+      <c r="D547" s="17">
+        <v>98</v>
+      </c>
+      <c r="E547">
+        <f t="shared" si="34"/>
+        <v>-41</v>
+      </c>
+      <c r="F547">
+        <f t="shared" si="35"/>
+        <v>0</v>
+      </c>
+      <c r="G547">
+        <f t="shared" si="36"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="548" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A548" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="B548" s="13">
+        <v>547</v>
+      </c>
+      <c r="C548" s="14">
+        <v>45919</v>
+      </c>
+      <c r="D548" s="17">
+        <v>151</v>
+      </c>
+      <c r="E548">
+        <f t="shared" si="34"/>
+        <v>-36.5</v>
+      </c>
+      <c r="F548">
+        <f t="shared" si="35"/>
+        <v>0</v>
+      </c>
+      <c r="G548">
+        <f t="shared" si="36"/>
+        <v>151</v>
+      </c>
+    </row>
+    <row r="549" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A549" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="B549" s="13">
+        <v>548</v>
+      </c>
+      <c r="C549" s="14">
+        <v>45920</v>
+      </c>
+      <c r="D549" s="17">
+        <v>171</v>
+      </c>
+      <c r="E549">
+        <f t="shared" si="34"/>
+        <v>39</v>
+      </c>
+      <c r="F549">
+        <f t="shared" si="35"/>
+        <v>171</v>
+      </c>
+      <c r="G549">
+        <f t="shared" si="36"/>
+        <v>171</v>
+      </c>
+    </row>
+    <row r="550" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A550" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="B550" s="13">
+        <v>549</v>
+      </c>
+      <c r="C550" s="14">
+        <v>45921</v>
+      </c>
+      <c r="D550" s="17">
+        <v>73</v>
+      </c>
+      <c r="E550">
+        <f t="shared" si="34"/>
+        <v>65</v>
+      </c>
+      <c r="F550">
+        <f t="shared" si="35"/>
+        <v>0</v>
+      </c>
+      <c r="G550">
+        <f t="shared" si="36"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="551" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A551" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="B551" s="13">
+        <v>550</v>
+      </c>
+      <c r="C551" s="14">
+        <v>45922</v>
+      </c>
+      <c r="D551" s="17">
+        <v>41</v>
+      </c>
+      <c r="E551">
+        <f t="shared" si="34"/>
+        <v>13</v>
+      </c>
+      <c r="F551">
+        <f t="shared" si="35"/>
+        <v>0</v>
+      </c>
+      <c r="G551">
+        <f t="shared" si="36"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="552" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A552" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="B552" s="13">
+        <v>551</v>
+      </c>
+      <c r="C552" s="14">
+        <v>45923</v>
+      </c>
+      <c r="D552" s="17">
+        <v>47</v>
+      </c>
+      <c r="E552">
+        <f t="shared" si="34"/>
+        <v>-13.5</v>
+      </c>
+      <c r="F552">
+        <f t="shared" si="35"/>
+        <v>0</v>
+      </c>
+      <c r="G552">
+        <f t="shared" si="36"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="553" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A553" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="B553" s="13">
+        <v>552</v>
+      </c>
+      <c r="C553" s="14">
+        <v>45924</v>
+      </c>
+      <c r="D553" s="17">
+        <v>68</v>
+      </c>
+      <c r="E553">
+        <f t="shared" si="34"/>
+        <v>-27</v>
+      </c>
+      <c r="F553">
+        <f t="shared" si="35"/>
+        <v>0</v>
+      </c>
+      <c r="G553">
+        <f t="shared" si="36"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="554" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A554" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="B554" s="13">
+        <v>553</v>
+      </c>
+      <c r="C554" s="14">
+        <v>45925</v>
+      </c>
+      <c r="D554" s="17">
+        <v>101</v>
+      </c>
+      <c r="E554">
+        <f t="shared" si="34"/>
+        <v>-45</v>
+      </c>
+      <c r="F554">
+        <f t="shared" si="35"/>
+        <v>0</v>
+      </c>
+      <c r="G554">
+        <f t="shared" si="36"/>
+        <v>101</v>
+      </c>
+    </row>
+    <row r="555" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A555" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="B555" s="13">
+        <v>554</v>
+      </c>
+      <c r="C555" s="14">
+        <v>45926</v>
+      </c>
+      <c r="D555" s="17">
+        <v>158</v>
+      </c>
+      <c r="E555">
+        <f t="shared" si="34"/>
+        <v>-44.5</v>
+      </c>
+      <c r="F555">
+        <f t="shared" si="35"/>
+        <v>0</v>
+      </c>
+      <c r="G555">
+        <f t="shared" si="36"/>
+        <v>158</v>
+      </c>
+    </row>
+    <row r="556" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A556" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="B556" s="13">
+        <v>555</v>
+      </c>
+      <c r="C556" s="14">
+        <v>45927</v>
+      </c>
+      <c r="D556" s="17">
+        <v>190</v>
+      </c>
+      <c r="E556">
+        <f t="shared" si="34"/>
+        <v>52.5</v>
+      </c>
+      <c r="F556">
+        <f t="shared" si="35"/>
+        <v>190</v>
+      </c>
+      <c r="G556">
+        <f t="shared" si="36"/>
+        <v>190</v>
+      </c>
+    </row>
+    <row r="557" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A557" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="B557" s="13">
+        <v>556</v>
+      </c>
+      <c r="C557" s="14">
+        <v>45928</v>
+      </c>
+      <c r="D557" s="17">
+        <v>53</v>
+      </c>
+      <c r="E557">
+        <f t="shared" si="34"/>
+        <v>76</v>
+      </c>
+      <c r="F557">
+        <f t="shared" si="35"/>
+        <v>0</v>
+      </c>
+      <c r="G557">
+        <f t="shared" si="36"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="558" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A558" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="B558" s="13">
+        <v>557</v>
+      </c>
+      <c r="C558" s="14">
+        <v>45929</v>
+      </c>
+      <c r="D558" s="17">
+        <v>38</v>
+      </c>
+      <c r="E558">
+        <f t="shared" si="34"/>
+        <v>-1</v>
+      </c>
+      <c r="F558">
+        <f t="shared" si="35"/>
+        <v>0</v>
+      </c>
+      <c r="G558">
+        <f t="shared" si="36"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="559" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A559" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="B559" s="13">
+        <v>558</v>
+      </c>
+      <c r="C559" s="14">
+        <v>45930</v>
+      </c>
+      <c r="D559" s="17">
+        <v>55</v>
+      </c>
+      <c r="E559">
+        <f t="shared" si="34"/>
+        <v>-18.5</v>
+      </c>
+      <c r="F559">
+        <f t="shared" si="35"/>
+        <v>0</v>
+      </c>
+      <c r="G559">
+        <f t="shared" si="36"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="560" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A560" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="B560" s="13">
+        <v>559</v>
+      </c>
+      <c r="C560" s="14">
+        <v>45931</v>
+      </c>
+      <c r="D560" s="17">
+        <v>75</v>
+      </c>
+      <c r="E560">
+        <f t="shared" si="34"/>
+        <v>-13.5</v>
+      </c>
+      <c r="F560">
+        <f t="shared" si="35"/>
+        <v>0</v>
+      </c>
+      <c r="G560">
+        <f t="shared" si="36"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="561" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A561" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="B561" s="13">
+        <v>560</v>
+      </c>
+      <c r="C561" s="14">
+        <v>45932</v>
+      </c>
+      <c r="D561" s="17">
+        <v>82</v>
+      </c>
+      <c r="E561">
+        <f t="shared" si="34"/>
+        <v>-34.5</v>
+      </c>
+      <c r="F561">
+        <f t="shared" si="35"/>
+        <v>0</v>
+      </c>
+      <c r="G561">
+        <f t="shared" si="36"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="562" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A562" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="B562" s="13">
+        <v>561</v>
+      </c>
+      <c r="C562" s="14">
+        <v>45933</v>
+      </c>
+      <c r="D562" s="17">
+        <v>144</v>
+      </c>
+      <c r="E562">
+        <f t="shared" si="34"/>
+        <v>-54</v>
+      </c>
+      <c r="F562">
+        <f t="shared" si="35"/>
+        <v>0</v>
+      </c>
+      <c r="G562">
+        <f t="shared" si="36"/>
+        <v>144</v>
+      </c>
+    </row>
+    <row r="563" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A563" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="B563" s="13">
+        <v>562</v>
+      </c>
+      <c r="C563" s="14">
+        <v>45934</v>
+      </c>
+      <c r="D563" s="17">
+        <v>190</v>
+      </c>
+      <c r="E563">
+        <f t="shared" si="34"/>
+        <v>47</v>
+      </c>
+      <c r="F563">
+        <f t="shared" si="35"/>
+        <v>190</v>
+      </c>
+      <c r="G563">
+        <f t="shared" si="36"/>
+        <v>190</v>
+      </c>
+    </row>
+    <row r="564" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A564" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="B564" s="13">
+        <v>563</v>
+      </c>
+      <c r="C564" s="14">
+        <v>45935</v>
+      </c>
+      <c r="D564" s="17">
+        <v>50</v>
+      </c>
+      <c r="E564">
+        <f t="shared" si="34"/>
+        <v>76</v>
+      </c>
+      <c r="F564">
+        <f t="shared" si="35"/>
+        <v>0</v>
+      </c>
+      <c r="G564">
+        <f t="shared" si="36"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="565" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A565" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="B565" s="13">
+        <v>564</v>
+      </c>
+      <c r="C565" s="14">
+        <v>45936</v>
+      </c>
+      <c r="D565" s="17">
+        <v>38</v>
+      </c>
+      <c r="E565">
+        <f t="shared" si="34"/>
+        <v>-27.5</v>
+      </c>
+      <c r="F565">
+        <f t="shared" si="35"/>
+        <v>0</v>
+      </c>
+      <c r="G565">
+        <f t="shared" si="36"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="566" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A566" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="B566" s="13">
+        <v>565</v>
+      </c>
+      <c r="C566" s="14">
+        <v>45937</v>
+      </c>
+      <c r="D566" s="20">
+        <v>105</v>
+      </c>
+      <c r="E566">
+        <f t="shared" si="34"/>
+        <v>0</v>
+      </c>
+      <c r="F566">
+        <f t="shared" si="35"/>
+        <v>105</v>
+      </c>
+      <c r="G566">
+        <f t="shared" si="36"/>
+        <v>105</v>
+      </c>
+    </row>
+    <row r="567" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A567" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="B567" s="13">
+        <v>566</v>
+      </c>
+      <c r="C567" s="14">
+        <v>45938</v>
+      </c>
+      <c r="D567" s="20">
+        <v>38</v>
+      </c>
+      <c r="E567">
+        <f t="shared" si="34"/>
+        <v>52.5</v>
+      </c>
+      <c r="F567">
+        <f t="shared" si="35"/>
+        <v>0</v>
+      </c>
+      <c r="G567">
+        <f t="shared" si="36"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="568" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A568" s="8"/>
+    </row>
+    <row r="569" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A569" s="8"/>
+    </row>
+    <row r="570" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A570" s="8"/>
+    </row>
+    <row r="571" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A571" s="8"/>
+    </row>
+    <row r="572" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A572" s="8"/>
+    </row>
+    <row r="573" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A573" s="8"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>